<commit_message>
1, retweet-network: selected most frequent tweets, add lorenz curve, changes titles; 2, download 1M followers' friends, may take 30 days
</commit_message>
<xml_diff>
--- a/Topics and Following clusters.xlsx
+++ b/Topics and Following clusters.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="184">
   <si>
     <t>topic #</t>
   </si>
@@ -132,7 +132,7 @@
     <t>unclear (daily life?)</t>
   </si>
   <si>
-    <t>TV </t>
+    <t>TV</t>
   </si>
   <si>
     <t>TV entertainment</t>
@@ -195,7 +195,7 @@
     <t>French</t>
   </si>
   <si>
-    <t>A cluster is defined and named based on the categories of accounts the particular cluster of people follow. (notes) [demographic] </t>
+    <t>A cluster is defined and named based on the categories of accounts the particular cluster of people follow. (notes) [demographic]</t>
   </si>
   <si>
     <t>Cluster #</t>
@@ -219,19 +219,25 @@
     <t>Trump campaign &amp; surrogates</t>
   </si>
   <si>
+    <t>TrumpCampaignSurrgts</t>
+  </si>
+  <si>
     <t>civic org. &amp; tech(Eng+arabic)</t>
   </si>
   <si>
     <t>conservative politicians and media [Trump supporters]</t>
   </si>
   <si>
-    <t>conservative politicians and media</t>
+    <t>TrumpCampaignConsvMedia</t>
   </si>
   <si>
     <t>conservative politicians, org. &amp; media</t>
   </si>
   <si>
-    <t>Trump family and surrogates </t>
+    <t>Trump family and surrogates</t>
+  </si>
+  <si>
+    <t>TrumpFamilySurrgts</t>
   </si>
   <si>
     <t>South Africa</t>
@@ -240,6 +246,9 @@
     <t>Trump family, business &amp; conservative media</t>
   </si>
   <si>
+    <t>TrumpFamilyBusinessConsvMedia</t>
+  </si>
+  <si>
     <t>gov. (international relations)(Eng+arabic)</t>
   </si>
   <si>
@@ -249,7 +258,7 @@
     <t>white nationalist media outlets (alt-right)</t>
   </si>
   <si>
-    <t>white nationalist media (alt-right)</t>
+    <t>WhiteNationalists</t>
   </si>
   <si>
     <t>politicians &amp; media (eng + spanish)</t>
@@ -261,13 +270,16 @@
     <t>conservative media and politicians</t>
   </si>
   <si>
+    <t>ConsvMediaPoliticians</t>
+  </si>
+  <si>
     <t>politicians, news (China + other foreign countries)</t>
   </si>
   <si>
     <t>Netherlands (follow more republican politicians)</t>
   </si>
   <si>
-    <t>Netherlands (republican politicians)</t>
+    <t>RepubPolitNetherland</t>
   </si>
   <si>
     <t>entertainment shows &amp; personalities [women]</t>
@@ -276,45 +288,63 @@
     <t>conservative media</t>
   </si>
   <si>
-    <t>liberal media </t>
+    <t>ConsvMedia</t>
+  </si>
+  <si>
+    <t>liberal media</t>
   </si>
   <si>
     <t>conservative politicians</t>
   </si>
   <si>
+    <t>ConsvPoliticians</t>
+  </si>
+  <si>
     <t>conservative politicians &amp; Florida [conservatives]</t>
   </si>
   <si>
-    <t>conservative politicians &amp; Florida</t>
-  </si>
-  <si>
-    <t>Chinese &amp; celebrity </t>
+    <t>ConsvPoliticians&amp;Fl</t>
+  </si>
+  <si>
+    <t>Chinese &amp; celebrity</t>
   </si>
   <si>
     <t>Liberals (politically engaged, interested in politics &amp; media)</t>
   </si>
   <si>
+    <t>LibMedia</t>
+  </si>
+  <si>
     <t>politicians, media, NASA</t>
   </si>
   <si>
     <t>liberal media &amp; politician</t>
   </si>
   <si>
+    <t>LibMediaPoliticians</t>
+  </si>
+  <si>
     <t>news people</t>
   </si>
   <si>
     <t>Australia, Netherlands, Belgium (follow more liberal politicians)</t>
   </si>
   <si>
-    <t>Australia, Netherlands (liberal politicians)</t>
+    <t>LibPolit&amp;OtherCountries</t>
   </si>
   <si>
     <t>Australia (follow more liberal politicians)</t>
   </si>
   <si>
+    <t>LibPolit&amp;Australia</t>
+  </si>
+  <si>
     <t>liberal politicians &amp; late night comedies</t>
   </si>
   <si>
+    <t>LibPolit&amp;Comedy</t>
+  </si>
+  <si>
     <t>politically engaged/GOP</t>
   </si>
   <si>
@@ -327,39 +357,63 @@
     <t>politicians &amp; media</t>
   </si>
   <si>
+    <t>Politicians&amp;Media</t>
+  </si>
+  <si>
     <t>gov. &amp; officials</t>
   </si>
   <si>
-    <t>politicians, news (China + other countries)</t>
+    <t>PoliticiansNewsOtherCountries</t>
+  </si>
+  <si>
+    <t>PoliticiansMediaNASA</t>
   </si>
   <si>
     <t>gov. &amp; politics &amp; media</t>
   </si>
   <si>
+    <t>PoliticiansNeutralMediaFinanceApple</t>
+  </si>
+  <si>
     <t>local news/FL,NJ etc</t>
   </si>
   <si>
     <t>Florida (Palm beach)</t>
   </si>
   <si>
+    <t>GovPoliticsMedia</t>
+  </si>
+  <si>
     <t>politically  right,indep</t>
   </si>
   <si>
     <t>politicians, gov., media, national park</t>
   </si>
   <si>
+    <t>PoliticiansGovMediaNationalPark</t>
+  </si>
+  <si>
     <t>political parties &amp; neutral media</t>
   </si>
   <si>
+    <t>Parties&amp;NeutralMedia</t>
+  </si>
+  <si>
     <t>celebrity, sports [probably millenials]</t>
   </si>
   <si>
     <t>Media junkies</t>
   </si>
   <si>
+    <t>MediaOutlets</t>
+  </si>
+  <si>
     <t>weather &amp; media junkie</t>
   </si>
   <si>
+    <t>Weather&amp;MediaOutlets</t>
+  </si>
+  <si>
     <t>India</t>
   </si>
   <si>
@@ -369,34 +423,46 @@
     <t>gov. (international relations)</t>
   </si>
   <si>
+    <t>Gov</t>
+  </si>
+  <si>
     <t>don't know (daily life, no politics)</t>
   </si>
   <si>
     <t>foreign media, tech, game</t>
   </si>
   <si>
+    <t>Gov&amp;Officials</t>
+  </si>
+  <si>
     <t>Finance &amp; economics &amp; parents [female parents, housewives]</t>
   </si>
   <si>
     <t>civic org. &amp; tech</t>
   </si>
   <si>
+    <t>CivicOrg&amp;Tech</t>
+  </si>
+  <si>
     <t>Youtubers [highly probably millenials]</t>
   </si>
   <si>
     <t>civic org &amp; lifestyle</t>
   </si>
   <si>
+    <t>CivicOrg&amp;Lifestyle</t>
+  </si>
+  <si>
     <t>Trump campaign, conservative politicians and media [Trump supporters]</t>
   </si>
   <si>
-    <t>entertainment celeb</t>
+    <t>Entertainment&amp;celeb</t>
   </si>
   <si>
     <t>entertainment shows &amp; celeb [women?]</t>
   </si>
   <si>
-    <t>entertainment shows &amp; celeb</t>
+    <t>TVShows&amp;Celeb</t>
   </si>
   <si>
     <t>science and technology</t>
@@ -405,19 +471,31 @@
     <t>celeb [probably millenials]</t>
   </si>
   <si>
+    <t>Celeb</t>
+  </si>
+  <si>
     <t>gov officials, agencies(some GOP)</t>
   </si>
   <si>
+    <t>Youtubers</t>
+  </si>
+  <si>
     <t>NASA &amp; Space</t>
   </si>
   <si>
+    <t>CelebSports</t>
+  </si>
+  <si>
     <t>sports &amp; football</t>
   </si>
   <si>
+    <t>SportsFootball</t>
+  </si>
+  <si>
     <t>Lifestyles</t>
   </si>
   <si>
-    <t>Finance &amp; economics &amp; parents</t>
+    <t>FinanceEconomyParents</t>
   </si>
   <si>
     <t>main stream leaders, international</t>
@@ -426,43 +504,70 @@
     <t>Lifestyle (food,arts,scenery etc)</t>
   </si>
   <si>
+    <t>Lifestyle</t>
+  </si>
+  <si>
     <t>social causes, arts</t>
   </si>
   <si>
-    <t>Lifestyle</t>
-  </si>
-  <si>
     <t>Arizona</t>
   </si>
   <si>
     <t>Sci-tech</t>
   </si>
   <si>
+    <t>SciTech</t>
+  </si>
+  <si>
+    <t>NASA&amp;Space</t>
+  </si>
+  <si>
     <t>Regional</t>
   </si>
   <si>
     <t>Florida (Palm beach), Atlantic city, and other places</t>
   </si>
   <si>
-    <t>Palm beach, Atlantic city, and other places</t>
-  </si>
-  <si>
-    <t>California, comedy, celebrities </t>
-  </si>
-  <si>
-    <t>international</t>
+    <t>PalmBeachAtlanticCityOther</t>
+  </si>
+  <si>
+    <t>California, comedy, celebrities</t>
+  </si>
+  <si>
+    <t>CA&amp;ComedyCeleb</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>SouthAfrica</t>
   </si>
   <si>
     <t>Nigeria</t>
   </si>
   <si>
-    <t>China &amp; celebrity </t>
+    <t>China &amp; celebrity</t>
+  </si>
+  <si>
+    <t>China&amp;Celeb</t>
+  </si>
+  <si>
+    <t>ForeignMediaTechGame</t>
   </si>
   <si>
     <t>kenya/peru</t>
   </si>
   <si>
+    <t>KenyaPeru</t>
+  </si>
+  <si>
     <t>Finland, Argintina</t>
+  </si>
+  <si>
+    <t>FinlandArgintina</t>
   </si>
   <si>
     <t>conservative pundits and media (white nationalist media outlets)</t>
@@ -588,7 +693,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -609,10 +714,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -622,10 +723,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -722,9 +819,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.5296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.5296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83333333333333"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1849,34 +1944,26 @@
   </sheetPr>
   <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I45" activeCellId="0" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.4555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.8888888888889"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="10.5296296296296"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.2592592592593"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.0703703703704"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.162962962963"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="34.6962962962963"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="41.6555555555556"/>
-    <col collapsed="false" hidden="false" max="17" min="13" style="0" width="10.5296296296296"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.662962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="10.5296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.83333333333333"/>
+    <col collapsed="false" hidden="false" max="10" min="2" style="0" width="8.83333333333333"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.337037037037"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="47.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.83333333333333"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0"/>
       <c r="C1" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="C2" s="0" t="s">
         <v>59</v>
@@ -1906,7 +1993,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
       <c r="B3" s="0" t="n">
         <v>734</v>
@@ -1917,7 +2004,7 @@
       <c r="D3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>64</v>
       </c>
       <c r="J3" s="1" t="n">
@@ -1927,7 +2014,7 @@
         <v>65</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M3" s="1" t="n">
         <v>769</v>
@@ -1935,7 +2022,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
       <c r="B4" s="0" t="n">
         <v>1083</v>
@@ -1944,17 +2031,17 @@
         <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="I4" s="3"/>
       <c r="J4" s="1" t="n">
         <v>25</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M4" s="1" t="n">
         <v>1158</v>
@@ -1964,26 +2051,26 @@
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
       <c r="B5" s="0" t="n">
         <v>1073</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="3"/>
       <c r="J5" s="1" t="n">
         <v>30</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M5" s="1" t="n">
         <v>1109</v>
@@ -1992,26 +2079,26 @@
       <c r="O5" s="4"/>
       <c r="S5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="6" t="n">
         <v>740</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="1" t="n">
         <v>35</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="M6" s="1" t="n">
         <v>640</v>
@@ -2020,7 +2107,7 @@
       <c r="O6" s="1"/>
       <c r="S6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
       <c r="B7" s="0" t="n">
         <v>1239</v>
@@ -2029,17 +2116,17 @@
         <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" s="5"/>
+        <v>76</v>
+      </c>
+      <c r="I7" s="3"/>
       <c r="J7" s="1" t="n">
         <v>43</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="M7" s="1" t="n">
         <v>546</v>
@@ -2048,18 +2135,18 @@
       <c r="O7" s="2"/>
       <c r="S7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0"/>
       <c r="D8" s="4"/>
-      <c r="I8" s="5"/>
+      <c r="I8" s="3"/>
       <c r="J8" s="1" t="n">
         <v>46</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M8" s="1" t="n">
         <v>1340</v>
@@ -2068,28 +2155,28 @@
       <c r="O8" s="2"/>
       <c r="S8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
-      <c r="B9" s="7" t="n">
+      <c r="B9" s="6" t="n">
         <v>797</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="J9" s="1" t="n">
         <v>3</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="M9" s="1" t="n">
         <v>1073</v>
@@ -2097,7 +2184,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
       <c r="B10" s="0" t="n">
         <v>2732</v>
@@ -2106,17 +2193,17 @@
         <v>7</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" s="5"/>
+        <v>84</v>
+      </c>
+      <c r="I10" s="3"/>
       <c r="J10" s="1" t="n">
         <v>18</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="M10" s="1" t="n">
         <v>1578</v>
@@ -2124,26 +2211,26 @@
       <c r="N10" s="1"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
-      <c r="B11" s="7" t="n">
+      <c r="B11" s="6" t="n">
         <v>998</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I11" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="I11" s="3"/>
       <c r="J11" s="1" t="n">
         <v>29</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="M11" s="1" t="n">
         <v>1930</v>
@@ -2151,7 +2238,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0"/>
       <c r="B12" s="0" t="n">
         <v>972</v>
@@ -2160,17 +2247,17 @@
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I12" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="I12" s="3"/>
       <c r="J12" s="1" t="n">
         <v>36</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="M12" s="1" t="n">
         <v>998</v>
@@ -2178,18 +2265,18 @@
       <c r="N12" s="1"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
       <c r="D13" s="4"/>
-      <c r="I13" s="5"/>
+      <c r="I13" s="3"/>
       <c r="J13" s="1" t="n">
         <v>49</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="M13" s="1" t="n">
         <v>323</v>
@@ -2197,28 +2284,28 @@
       <c r="N13" s="1"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0"/>
-      <c r="B14" s="7" t="n">
+      <c r="B14" s="6" t="n">
         <v>1505</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>90</v>
+        <v>95</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J14" s="1" t="n">
         <v>9</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="M14" s="1" t="n">
         <v>972</v>
@@ -2226,26 +2313,26 @@
       <c r="N14" s="1"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0"/>
-      <c r="B15" s="8" t="n">
+      <c r="B15" s="7" t="n">
         <v>1773</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>11</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I15" s="5"/>
+        <v>98</v>
+      </c>
+      <c r="I15" s="3"/>
       <c r="J15" s="1" t="n">
         <v>12</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="M15" s="1" t="n">
         <v>1125</v>
@@ -2253,28 +2340,28 @@
       <c r="N15" s="1"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="7" t="n">
+    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="6" t="n">
         <v>1125</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="I16" s="5"/>
+        <v>99</v>
+      </c>
+      <c r="I16" s="3"/>
       <c r="J16" s="1" t="n">
         <v>19</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="M16" s="1" t="n">
         <v>852</v>
@@ -2282,19 +2369,19 @@
       <c r="N16" s="1"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9"/>
-      <c r="B17" s="7"/>
+    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
       <c r="D17" s="4"/>
-      <c r="I17" s="5"/>
+      <c r="I17" s="3"/>
       <c r="J17" s="1" t="n">
         <v>31</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="M17" s="1" t="n">
         <v>2150</v>
@@ -2302,19 +2389,19 @@
       <c r="N17" s="1"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9"/>
-      <c r="B18" s="7"/>
+    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
       <c r="D18" s="4"/>
-      <c r="I18" s="5"/>
+      <c r="I18" s="3"/>
       <c r="J18" s="1" t="n">
         <v>38</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="M18" s="1" t="n">
         <v>916</v>
@@ -2322,9 +2409,9 @@
       <c r="N18" s="1"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1781</v>
@@ -2333,19 +2420,19 @@
         <v>13</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>100</v>
+        <v>109</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="J19" s="1" t="n">
         <v>6</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="M19" s="1" t="n">
         <v>797</v>
@@ -2353,25 +2440,25 @@
       <c r="N19" s="1"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0"/>
-      <c r="B20" s="7" t="n">
+      <c r="B20" s="6" t="n">
         <v>457</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>14</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="J20" s="0" t="n">
         <v>7</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="M20" s="1" t="n">
         <v>2732</v>
@@ -2379,7 +2466,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
       <c r="B21" s="0" t="n">
         <v>769</v>
@@ -2387,18 +2474,18 @@
       <c r="C21" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I21" s="5"/>
+      <c r="I21" s="3"/>
       <c r="J21" s="1" t="n">
         <v>11</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="M21" s="1" t="n">
         <v>1773</v>
@@ -2406,26 +2493,26 @@
       <c r="N21" s="1"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>
-      <c r="B22" s="7" t="n">
+      <c r="B22" s="6" t="n">
         <v>812</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>16</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="I22" s="5"/>
+        <v>116</v>
+      </c>
+      <c r="I22" s="3"/>
       <c r="J22" s="0" t="n">
         <v>13</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="M22" s="0" t="n">
         <v>1781</v>
@@ -2433,9 +2520,9 @@
       <c r="N22" s="1"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>2528</v>
@@ -2444,17 +2531,17 @@
         <v>17</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="I23" s="5"/>
+        <v>119</v>
+      </c>
+      <c r="I23" s="3"/>
       <c r="J23" s="1" t="n">
         <v>16</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="M23" s="1" t="n">
         <v>812</v>
@@ -2462,28 +2549,28 @@
       <c r="N23" s="1"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B24" s="7" t="n">
+        <v>121</v>
+      </c>
+      <c r="B24" s="6" t="n">
         <v>1578</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>18</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I24" s="5"/>
+        <v>85</v>
+      </c>
+      <c r="I24" s="3"/>
       <c r="J24" s="1" t="n">
         <v>27</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="M24" s="1" t="n">
         <v>505</v>
@@ -2491,7 +2578,7 @@
       <c r="N24" s="1"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
       <c r="B25" s="0" t="n">
         <v>852</v>
@@ -2500,17 +2587,17 @@
         <v>19</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I25" s="5"/>
+        <v>102</v>
+      </c>
+      <c r="I25" s="3"/>
       <c r="J25" s="1" t="n">
         <v>34</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="M25" s="1" t="n">
         <v>815</v>
@@ -2518,26 +2605,26 @@
       <c r="N25" s="1"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0"/>
-      <c r="B26" s="7" t="n">
+      <c r="B26" s="6" t="n">
         <v>4214</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1" t="n">
         <v>37</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="M26" s="1" t="n">
         <v>1577</v>
@@ -2545,19 +2632,19 @@
       <c r="N26" s="1"/>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
-      <c r="B27" s="7"/>
+      <c r="B27" s="6"/>
       <c r="D27" s="4"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1" t="n">
         <v>40</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="M27" s="1" t="n">
         <v>1358</v>
@@ -2565,7 +2652,7 @@
       <c r="N27" s="1"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
       <c r="B28" s="0" t="n">
         <v>1522</v>
@@ -2574,19 +2661,19 @@
         <v>21</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>114</v>
+        <v>131</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="J28" s="1" t="n">
         <v>5</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="M28" s="1" t="n">
         <v>1239</v>
@@ -2594,28 +2681,28 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B29" s="7" t="n">
+        <v>135</v>
+      </c>
+      <c r="B29" s="6" t="n">
         <v>1954</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>22</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="I29" s="5"/>
+        <v>136</v>
+      </c>
+      <c r="I29" s="3"/>
       <c r="J29" s="1" t="n">
         <v>14</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="M29" s="1" t="n">
         <v>457</v>
@@ -2623,7 +2710,7 @@
       <c r="N29" s="1"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
       <c r="B30" s="0" t="n">
         <v>2836</v>
@@ -2632,17 +2719,17 @@
         <v>23</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="I30" s="5"/>
+        <v>138</v>
+      </c>
+      <c r="I30" s="3"/>
       <c r="J30" s="1" t="n">
         <v>2</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="M30" s="1" t="n">
         <v>1083</v>
@@ -2650,26 +2737,26 @@
       <c r="N30" s="1"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
-      <c r="B31" s="7" t="n">
+      <c r="B31" s="6" t="n">
         <v>2223</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>24</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="I31" s="5"/>
+        <v>141</v>
+      </c>
+      <c r="I31" s="3"/>
       <c r="J31" s="1" t="n">
         <v>42</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="M31" s="1" t="n">
         <v>840</v>
@@ -2677,7 +2764,7 @@
       <c r="N31" s="1"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
       <c r="B32" s="0" t="n">
         <v>1158</v>
@@ -2686,19 +2773,19 @@
         <v>25</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="J32" s="1" t="n">
         <v>8</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="M32" s="1" t="n">
         <v>998</v>
@@ -2706,25 +2793,25 @@
       <c r="N32" s="1"/>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="7" t="n">
+      <c r="B33" s="6" t="n">
         <v>1115</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>26</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="J33" s="1" t="n">
         <v>20</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="M33" s="1" t="n">
         <v>4214</v>
@@ -2732,9 +2819,9 @@
       <c r="N33" s="1"/>
       <c r="O33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>505</v>
@@ -2743,16 +2830,16 @@
         <v>27</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="J34" s="1" t="n">
         <v>24</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="M34" s="1" t="n">
         <v>2223</v>
@@ -2760,25 +2847,25 @@
       <c r="N34" s="1"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
-      <c r="B35" s="7" t="n">
+      <c r="B35" s="6" t="n">
         <v>424</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>28</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="J35" s="1" t="n">
         <v>44</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>110</v>
+        <v>154</v>
       </c>
       <c r="M35" s="1" t="n">
         <v>4435</v>
@@ -2786,7 +2873,7 @@
       <c r="N35" s="1"/>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0"/>
       <c r="B36" s="0" t="n">
         <v>1930</v>
@@ -2795,7 +2882,7 @@
         <v>29</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="I36" s="0" t="s">
         <v>25</v>
@@ -2804,10 +2891,10 @@
         <v>41</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="M36" s="1" t="n">
         <v>5181</v>
@@ -2815,28 +2902,28 @@
       <c r="N36" s="1"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
-      <c r="B37" s="7" t="n">
+      <c r="B37" s="6" t="n">
         <v>1109</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>30</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="J37" s="1" t="n">
         <v>23</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="M37" s="1" t="n">
         <v>2836</v>
@@ -2844,9 +2931,9 @@
       <c r="N37" s="1"/>
       <c r="O37" s="2"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>2150</v>
@@ -2855,16 +2942,16 @@
         <v>31</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="J38" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="K38" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="L38" s="10" t="s">
-        <v>134</v>
+      <c r="K38" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="L38" s="8" t="s">
+        <v>161</v>
       </c>
       <c r="M38" s="1" t="n">
         <v>1269</v>
@@ -2872,27 +2959,27 @@
       <c r="N38" s="1"/>
       <c r="O38" s="2"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B39" s="7" t="n">
+    <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B39" s="6" t="n">
         <v>1269</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="D39" s="10" t="s">
-        <v>134</v>
+      <c r="D39" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="J39" s="1" t="n">
         <v>45</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="M39" s="1" t="n">
         <v>1401</v>
@@ -2900,7 +2987,7 @@
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="n">
         <v>436</v>
       </c>
@@ -2908,19 +2995,19 @@
         <v>33</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="J40" s="1" t="n">
         <v>26</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>126</v>
+        <v>165</v>
       </c>
       <c r="M40" s="1" t="n">
         <v>1115</v>
@@ -2928,24 +3015,24 @@
       <c r="N40" s="1"/>
       <c r="O40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="7" t="n">
+    <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="6" t="n">
         <v>815</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>34</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="J41" s="1" t="n">
         <v>28</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="M41" s="1" t="n">
         <v>424</v>
@@ -2953,7 +3040,7 @@
       <c r="N41" s="1"/>
       <c r="O41" s="2"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="n">
         <v>640</v>
       </c>
@@ -2961,19 +3048,19 @@
         <v>35</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>139</v>
+        <v>74</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="J42" s="1" t="n">
         <v>17</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="M42" s="1" t="n">
         <v>2528</v>
@@ -2981,16 +3068,16 @@
       <c r="N42" s="1"/>
       <c r="O42" s="2"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D43" s="4"/>
       <c r="J43" s="1" t="n">
         <v>33</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="M43" s="1" t="n">
         <v>436</v>
@@ -2998,25 +3085,25 @@
       <c r="N43" s="1"/>
       <c r="O43" s="2"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="7" t="n">
+    <row r="44" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="6" t="n">
         <v>998</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>36</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I44" s="5"/>
+        <v>91</v>
+      </c>
+      <c r="I44" s="3"/>
       <c r="J44" s="1" t="n">
         <v>48</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="M44" s="1" t="n">
         <v>2332</v>
@@ -3024,7 +3111,7 @@
       <c r="N44" s="1"/>
       <c r="O44" s="2"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="n">
         <v>1577</v>
       </c>
@@ -3032,10 +3119,10 @@
         <v>37</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>143</v>
+        <v>127</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="J45" s="1" t="n">
         <v>1</v>
@@ -3044,7 +3131,7 @@
         <v>52</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="M45" s="1" t="n">
         <v>734</v>
@@ -3052,25 +3139,25 @@
       <c r="N45" s="1"/>
       <c r="O45" s="2"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="7" t="n">
+    <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="6" t="n">
         <v>916</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>38</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1" t="n">
         <v>4</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>71</v>
+        <v>174</v>
       </c>
       <c r="M46" s="1" t="n">
         <v>740</v>
@@ -3078,7 +3165,7 @@
       <c r="N46" s="1"/>
       <c r="O46" s="2"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="n">
         <v>1430</v>
       </c>
@@ -3086,17 +3173,17 @@
         <v>39</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>144</v>
+        <v>175</v>
       </c>
       <c r="I47" s="1"/>
       <c r="J47" s="1" t="n">
         <v>10</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="M47" s="1" t="n">
         <v>1505</v>
@@ -3104,25 +3191,25 @@
       <c r="N47" s="1"/>
       <c r="O47" s="2"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="7" t="n">
+    <row r="48" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="6" t="n">
         <v>1358</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>40</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" s="1" t="n">
         <v>21</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="M48" s="1" t="n">
         <v>1522</v>
@@ -3130,7 +3217,7 @@
       <c r="N48" s="1"/>
       <c r="O48" s="2"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="n">
         <v>5181</v>
       </c>
@@ -3138,17 +3225,17 @@
         <v>41</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="I49" s="1"/>
       <c r="J49" s="1" t="n">
         <v>22</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="M49" s="1" t="n">
         <v>1954</v>
@@ -3156,25 +3243,25 @@
       <c r="N49" s="1"/>
       <c r="O49" s="2"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="7" t="n">
+    <row r="50" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="6" t="n">
         <v>840</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>42</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="I50" s="1"/>
       <c r="J50" s="1" t="n">
         <v>39</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>144</v>
+        <v>175</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>144</v>
+        <v>175</v>
       </c>
       <c r="M50" s="1" t="n">
         <v>1430</v>
@@ -3182,7 +3269,7 @@
       <c r="N50" s="1"/>
       <c r="O50" s="2"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="n">
         <v>546</v>
       </c>
@@ -3190,17 +3277,17 @@
         <v>43</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="1" t="n">
         <v>47</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>146</v>
+        <v>179</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="M51" s="1" t="n">
         <v>3260</v>
@@ -3208,25 +3295,25 @@
       <c r="N51" s="1"/>
       <c r="O51" s="2"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="7" t="n">
+    <row r="52" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="6" t="n">
         <v>4435</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>44</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="I52" s="1"/>
       <c r="J52" s="1" t="n">
         <v>50</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>147</v>
+        <v>181</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="M52" s="1" t="n">
         <v>2153</v>
@@ -3234,7 +3321,7 @@
       <c r="N52" s="1"/>
       <c r="O52" s="2"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="n">
         <v>1401</v>
       </c>
@@ -3242,27 +3329,27 @@
         <v>45</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="I53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="2"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="7" t="n">
+    <row r="54" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="6" t="n">
         <v>1340</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>46</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
       <c r="I54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="2"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="n">
         <v>3260</v>
       </c>
@@ -3270,27 +3357,27 @@
         <v>47</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>146</v>
+        <v>179</v>
       </c>
       <c r="I55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="2"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="7" t="n">
+    <row r="56" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="6" t="n">
         <v>2332</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>48</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="I56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="2"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="n">
         <v>323</v>
       </c>
@@ -3298,20 +3385,20 @@
         <v>49</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="N57" s="1"/>
       <c r="O57" s="2"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="7" t="n">
+    <row r="58" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="6" t="n">
         <v>2153</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>50</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>147</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>